<commit_message>
set map default location
</commit_message>
<xml_diff>
--- a/docs/香港素食餐廳大全.xlsx
+++ b/docs/香港素食餐廳大全.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tim/_Python_OpenAI/My-projects/7-hk-veg-map/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5A0223-E896-D24E-B960-75F5A07B1CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FD4816-5D0E-DA40-BD57-E4F7B61ECAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="500" windowWidth="14640" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12660" yWindow="500" windowWidth="15000" windowHeight="16260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="香港素食餐廳大全" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="735">
   <si>
     <t>** 更新自: 13 Aug 2023 (deprecated, go to sheet 2 "hk_veg_restaurants_data instead")</t>
   </si>
@@ -2187,13 +2187,52 @@
   </si>
   <si>
     <t>22.284950391487587, 114.1537815780751</t>
+  </si>
+  <si>
+    <t>一素店</t>
+  </si>
+  <si>
+    <t>素一素</t>
+  </si>
+  <si>
+    <t xml:space="preserve">荔枝角 </t>
+  </si>
+  <si>
+    <t>Tempura Makino</t>
+  </si>
+  <si>
+    <t>寶光齋素食館</t>
+  </si>
+  <si>
+    <t>寶蓮禪寺</t>
+  </si>
+  <si>
+    <t>VEDA</t>
+  </si>
+  <si>
+    <t>一森素食</t>
+  </si>
+  <si>
+    <t>油麻地</t>
+  </si>
+  <si>
+    <t>素之苑</t>
+  </si>
+  <si>
+    <t>So Coco</t>
+  </si>
+  <si>
+    <t>樂園素食</t>
+  </si>
+  <si>
+    <t>Veggie4love</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2277,6 +2316,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -2328,7 +2374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2357,6 +2403,7 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10434,10 +10481,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -10950,30 +10997,18 @@
         <v>10</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>436</v>
-      </c>
+        <v>728</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>437</v>
-      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="5"/>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
@@ -10981,30 +11016,18 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>439</v>
-      </c>
+        <v>734</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="6" t="s">
-        <v>440</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>441</v>
-      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="23"/>
       <c r="K18" s="5"/>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
@@ -11012,29 +11035,29 @@
         <v>10</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>71</v>
+        <v>411</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>72</v>
+        <v>435</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="K19" s="5"/>
     </row>
@@ -11043,29 +11066,29 @@
         <v>10</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>74</v>
+        <v>381</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>75</v>
+        <v>382</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>76</v>
+        <v>438</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="I20" s="7" t="s">
-        <v>77</v>
+      <c r="I20" s="6" t="s">
+        <v>440</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="K20" s="5"/>
     </row>
@@ -11077,26 +11100,26 @@
         <v>69</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>394</v>
+        <v>71</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="7" t="s">
-        <v>80</v>
+      <c r="I21" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="K21" s="5"/>
     </row>
@@ -11108,26 +11131,26 @@
         <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>411</v>
+        <v>75</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="K22" s="5"/>
     </row>
@@ -11139,26 +11162,26 @@
         <v>69</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>411</v>
+        <v>394</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="H23" s="5"/>
-      <c r="I23" s="6" t="s">
-        <v>86</v>
+      <c r="I23" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="K23" s="5"/>
     </row>
@@ -11170,7 +11193,7 @@
         <v>69</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>411</v>
@@ -11179,17 +11202,17 @@
         <v>25</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="6" t="s">
-        <v>89</v>
+      <c r="I24" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K24" s="5"/>
     </row>
@@ -11201,26 +11224,26 @@
         <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>51</v>
+        <v>411</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="K25" s="5"/>
     </row>
@@ -11232,26 +11255,26 @@
         <v>69</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>55</v>
+        <v>411</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="K26" s="5"/>
     </row>
@@ -11263,26 +11286,26 @@
         <v>69</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>419</v>
+        <v>51</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="K27" s="5"/>
     </row>
@@ -11291,29 +11314,29 @@
         <v>10</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>460</v>
+        <v>93</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>411</v>
+        <v>55</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>461</v>
+        <v>94</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="6" t="s">
-        <v>463</v>
+        <v>95</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="K28" s="5"/>
     </row>
@@ -11322,29 +11345,29 @@
         <v>10</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>381</v>
+        <v>96</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>382</v>
+        <v>419</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>465</v>
+        <v>97</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="6" t="s">
-        <v>467</v>
+        <v>98</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="K29" s="5"/>
     </row>
@@ -11356,30 +11379,28 @@
         <v>99</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>100</v>
+        <v>460</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>47</v>
+        <v>411</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>101</v>
+        <v>461</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="6" t="s">
-        <v>102</v>
+        <v>463</v>
       </c>
       <c r="J30" s="23" t="s">
-        <v>470</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>103</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="K30" s="5"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="A31" s="5" t="s">
@@ -11389,26 +11410,26 @@
         <v>99</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>104</v>
+        <v>381</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>471</v>
+        <v>382</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>106</v>
+        <v>465</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="7" t="s">
-        <v>107</v>
+      <c r="I31" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="K31" s="5"/>
     </row>
@@ -11420,28 +11441,30 @@
         <v>99</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>474</v>
+        <v>47</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>475</v>
+        <v>101</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="6" t="s">
-        <v>477</v>
+        <v>102</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>478</v>
-      </c>
-      <c r="K32" s="5"/>
+        <v>470</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
       <c r="A33" s="5" t="s">
@@ -11451,26 +11474,26 @@
         <v>99</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>55</v>
+        <v>471</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="H33" s="5"/>
-      <c r="I33" s="6" t="s">
-        <v>114</v>
+      <c r="I33" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="K33" s="5"/>
     </row>
@@ -11479,29 +11502,29 @@
         <v>10</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>481</v>
+        <v>108</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>47</v>
+        <v>474</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="6" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="K34" s="5"/>
     </row>
@@ -11510,29 +11533,29 @@
         <v>10</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="K35" s="5"/>
     </row>
@@ -11541,61 +11564,37 @@
         <v>10</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>488</v>
-      </c>
+        <v>732</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="J36" s="23" t="s">
-        <v>489</v>
-      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="23"/>
       <c r="K36" s="5"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>124</v>
+      <c r="B37" s="26" t="s">
+        <v>99</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>490</v>
-      </c>
+        <v>733</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J37" s="23" t="s">
-        <v>491</v>
-      </c>
+      <c r="I37" s="6"/>
+      <c r="J37" s="23"/>
       <c r="K37" s="5"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
@@ -11603,155 +11602,155 @@
         <v>10</v>
       </c>
       <c r="B38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="J38" s="23" t="s">
+        <v>485</v>
+      </c>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="H39" s="5"/>
+      <c r="I39" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="J39" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J40" s="23" t="s">
+        <v>489</v>
+      </c>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A41" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>491</v>
+      </c>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="5" t="s">
+      <c r="E42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G42" s="5" t="s">
         <v>492</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="7" t="s">
+      <c r="H42" s="5"/>
+      <c r="I42" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="J42" s="23" t="s">
         <v>493</v>
       </c>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A39" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="H39" s="9"/>
-      <c r="I39" s="10" t="s">
-        <v>497</v>
-      </c>
-      <c r="J39" s="24" t="s">
-        <v>498</v>
-      </c>
-      <c r="K39" s="9"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>499</v>
-      </c>
-      <c r="H40" s="9"/>
-      <c r="I40" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="J40" s="24" t="s">
-        <v>500</v>
-      </c>
-      <c r="K40" s="9"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A41" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>503</v>
-      </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="10" t="s">
-        <v>504</v>
-      </c>
-      <c r="J41" s="24" t="s">
-        <v>505</v>
-      </c>
-      <c r="K41" s="9"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A42" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="H42" s="9"/>
-      <c r="I42" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="J42" s="24" t="s">
-        <v>507</v>
-      </c>
-      <c r="K42" s="9"/>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" s="9" t="s">
@@ -11761,26 +11760,26 @@
         <v>133</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>381</v>
+        <v>494</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>382</v>
+        <v>47</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>509</v>
+        <v>496</v>
       </c>
       <c r="H43" s="9"/>
       <c r="I43" s="10" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="J43" s="24" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="K43" s="9"/>
     </row>
@@ -11792,26 +11791,26 @@
         <v>133</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>75</v>
+        <v>411</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="H44" s="9"/>
       <c r="I44" s="10" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="J44" s="24" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="K44" s="9"/>
     </row>
@@ -11823,26 +11822,26 @@
         <v>133</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>143</v>
+        <v>501</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>75</v>
+        <v>411</v>
       </c>
       <c r="E45" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>144</v>
+        <v>502</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="H45" s="9"/>
-      <c r="I45" s="11" t="s">
-        <v>145</v>
+      <c r="I45" s="10" t="s">
+        <v>504</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="K45" s="9"/>
     </row>
@@ -11854,30 +11853,30 @@
         <v>133</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>516</v>
+        <v>474</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="H46" s="9"/>
-      <c r="I46" s="11" t="s">
-        <v>149</v>
+      <c r="I46" s="10" t="s">
+        <v>139</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>518</v>
+        <v>507</v>
       </c>
       <c r="K46" s="9"/>
     </row>
-    <row r="47" spans="1:11" ht="13">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="A47" s="9" t="s">
         <v>132</v>
       </c>
@@ -11885,30 +11884,30 @@
         <v>133</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>150</v>
+        <v>381</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>55</v>
+        <v>382</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>151</v>
+        <v>508</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="H47" s="9"/>
       <c r="I47" s="10" t="s">
-        <v>152</v>
+        <v>510</v>
       </c>
       <c r="J47" s="24" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="K47" s="9"/>
     </row>
-    <row r="48" spans="1:11" ht="13">
+    <row r="48" spans="1:11" ht="15.75" customHeight="1">
       <c r="A48" s="9" t="s">
         <v>132</v>
       </c>
@@ -11916,7 +11915,7 @@
         <v>133</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>75</v>
@@ -11925,21 +11924,21 @@
         <v>25</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="H48" s="9"/>
       <c r="I48" s="10" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="J48" s="24" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="K48" s="9"/>
     </row>
-    <row r="49" spans="1:11" ht="13">
+    <row r="49" spans="1:11" ht="15.75" customHeight="1">
       <c r="A49" s="9" t="s">
         <v>132</v>
       </c>
@@ -11947,30 +11946,30 @@
         <v>133</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>157</v>
+        <v>75</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="H49" s="9"/>
-      <c r="I49" s="10" t="s">
-        <v>159</v>
+      <c r="I49" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="J49" s="24" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="K49" s="9"/>
     </row>
-    <row r="50" spans="1:11" ht="13">
+    <row r="50" spans="1:11" ht="15.75" customHeight="1">
       <c r="A50" s="9" t="s">
         <v>132</v>
       </c>
@@ -11978,26 +11977,26 @@
         <v>133</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>55</v>
+        <v>516</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="H50" s="9"/>
-      <c r="I50" s="10" t="s">
-        <v>162</v>
+      <c r="I50" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="J50" s="24" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="K50" s="9"/>
     </row>
@@ -12006,29 +12005,29 @@
         <v>132</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>411</v>
+        <v>55</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="H51" s="9"/>
       <c r="I51" s="10" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="J51" s="24" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="K51" s="9"/>
     </row>
@@ -12037,29 +12036,29 @@
         <v>132</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>411</v>
+        <v>75</v>
       </c>
       <c r="E52" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="H52" s="9"/>
       <c r="I52" s="10" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="J52" s="24" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="K52" s="9"/>
     </row>
@@ -12068,29 +12067,29 @@
         <v>132</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="E53" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="H53" s="9"/>
       <c r="I53" s="10" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="J53" s="24" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="K53" s="9"/>
     </row>
@@ -12099,29 +12098,29 @@
         <v>132</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="E54" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="H54" s="9"/>
       <c r="I54" s="10" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="J54" s="24" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="K54" s="9"/>
     </row>
@@ -12130,29 +12129,29 @@
         <v>132</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>535</v>
+        <v>163</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>536</v>
+        <v>164</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>157</v>
+        <v>411</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>537</v>
+        <v>165</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="H55" s="9"/>
-      <c r="I55" s="11" t="s">
-        <v>539</v>
+      <c r="I55" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="J55" s="24" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="K55" s="9"/>
     </row>
@@ -12161,29 +12160,29 @@
         <v>132</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>535</v>
+        <v>163</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>381</v>
+        <v>167</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>382</v>
+        <v>411</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>541</v>
+        <v>168</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="H56" s="9"/>
       <c r="I56" s="10" t="s">
-        <v>543</v>
+        <v>169</v>
       </c>
       <c r="J56" s="24" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="K56" s="9"/>
     </row>
@@ -12192,29 +12191,29 @@
         <v>132</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>545</v>
+        <v>170</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>411</v>
+        <v>117</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>546</v>
+        <v>171</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="H57" s="9"/>
       <c r="I57" s="10" t="s">
-        <v>548</v>
+        <v>172</v>
       </c>
       <c r="J57" s="24" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
       <c r="K57" s="9"/>
     </row>
@@ -12223,29 +12222,29 @@
         <v>132</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>411</v>
+        <v>117</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>550</v>
+        <v>174</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>551</v>
+        <v>533</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="10" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J58" s="24" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="K58" s="9"/>
     </row>
@@ -12254,30 +12253,18 @@
         <v>132</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>176</v>
+        <v>730</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G59" s="9" t="s">
-        <v>553</v>
-      </c>
+        <v>729</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="J59" s="24" t="s">
-        <v>554</v>
-      </c>
+      <c r="I59" s="10"/>
+      <c r="J59" s="24"/>
       <c r="K59" s="9"/>
     </row>
     <row r="60" spans="1:11" ht="13">
@@ -12285,29 +12272,29 @@
         <v>132</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>184</v>
+        <v>535</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>185</v>
+        <v>536</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>411</v>
+        <v>157</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>186</v>
+        <v>537</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>555</v>
+        <v>538</v>
       </c>
       <c r="H60" s="9"/>
-      <c r="I60" s="10" t="s">
-        <v>187</v>
+      <c r="I60" s="11" t="s">
+        <v>539</v>
       </c>
       <c r="J60" s="24" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="K60" s="9"/>
     </row>
@@ -12316,29 +12303,29 @@
         <v>132</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>184</v>
+        <v>535</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>188</v>
+        <v>381</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>117</v>
+        <v>382</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>189</v>
+        <v>541</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>557</v>
+        <v>542</v>
       </c>
       <c r="H61" s="9"/>
       <c r="I61" s="10" t="s">
-        <v>190</v>
+        <v>543</v>
       </c>
       <c r="J61" s="24" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="K61" s="9"/>
     </row>
@@ -12347,29 +12334,29 @@
         <v>132</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>191</v>
+        <v>545</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>192</v>
+        <v>411</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>193</v>
+        <v>546</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="10" t="s">
-        <v>194</v>
+        <v>548</v>
       </c>
       <c r="J62" s="24" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="K62" s="9"/>
     </row>
@@ -12378,29 +12365,29 @@
         <v>132</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>51</v>
+        <v>411</v>
       </c>
       <c r="E63" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>196</v>
+        <v>550</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="10" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="J63" s="24" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="K63" s="9"/>
     </row>
@@ -12409,29 +12396,29 @@
         <v>132</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>419</v>
+        <v>181</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="10" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="J64" s="24" t="s">
-        <v>564</v>
+        <v>554</v>
       </c>
       <c r="K64" s="9"/>
     </row>
@@ -12443,26 +12430,26 @@
         <v>184</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>565</v>
+        <v>555</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="10" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="J65" s="24" t="s">
-        <v>566</v>
+        <v>556</v>
       </c>
       <c r="K65" s="9"/>
     </row>
@@ -12473,27 +12460,27 @@
       <c r="B66" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C66" s="12" t="s">
-        <v>204</v>
+      <c r="C66" s="9" t="s">
+        <v>188</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>419</v>
+        <v>117</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>567</v>
+        <v>557</v>
       </c>
       <c r="H66" s="9"/>
-      <c r="I66" s="11" t="s">
-        <v>206</v>
+      <c r="I66" s="10" t="s">
+        <v>190</v>
       </c>
       <c r="J66" s="24" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="K66" s="9"/>
     </row>
@@ -12504,27 +12491,27 @@
       <c r="B67" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C67" s="12" t="s">
-        <v>207</v>
+      <c r="C67" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>419</v>
+        <v>192</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>569</v>
+        <v>559</v>
       </c>
       <c r="H67" s="9"/>
-      <c r="I67" s="11" t="s">
-        <v>209</v>
+      <c r="I67" s="10" t="s">
+        <v>194</v>
       </c>
       <c r="J67" s="24" t="s">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="K67" s="9"/>
     </row>
@@ -12533,29 +12520,29 @@
         <v>132</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>211</v>
+        <v>184</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>419</v>
+        <v>51</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>571</v>
+        <v>561</v>
       </c>
       <c r="H68" s="9"/>
       <c r="I68" s="10" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="J68" s="24" t="s">
-        <v>572</v>
+        <v>562</v>
       </c>
       <c r="K68" s="9"/>
     </row>
@@ -12564,29 +12551,29 @@
         <v>132</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>215</v>
+        <v>184</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>198</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>47</v>
+        <v>419</v>
       </c>
       <c r="E69" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>573</v>
+        <v>563</v>
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="10" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="J69" s="24" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="K69" s="9"/>
     </row>
@@ -12595,29 +12582,29 @@
         <v>132</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>218</v>
+        <v>184</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>157</v>
+        <v>419</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>575</v>
+        <v>565</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="10" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="J70" s="24" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="K70" s="9"/>
     </row>
@@ -12626,29 +12613,29 @@
         <v>132</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>577</v>
+        <v>204</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="H71" s="9"/>
-      <c r="I71" s="10" t="s">
-        <v>579</v>
+      <c r="I71" s="11" t="s">
+        <v>206</v>
       </c>
       <c r="J71" s="24" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="K71" s="9"/>
     </row>
@@ -12657,29 +12644,29 @@
         <v>132</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
       <c r="C72" s="12" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="D72" s="9" t="s">
         <v>419</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="H72" s="9"/>
-      <c r="I72" s="10" t="s">
-        <v>228</v>
+      <c r="I72" s="11" t="s">
+        <v>209</v>
       </c>
       <c r="J72" s="24" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="K72" s="9"/>
     </row>
@@ -12688,29 +12675,29 @@
         <v>132</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="H73" s="9"/>
       <c r="I73" s="10" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="J73" s="24" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="K73" s="9"/>
     </row>
@@ -12719,30 +12706,18 @@
         <v>132</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="C74" s="9" t="s">
-        <v>586</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>411</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>587</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>588</v>
-      </c>
+        <v>724</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>723</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
       <c r="H74" s="9"/>
-      <c r="I74" s="11" t="s">
-        <v>589</v>
-      </c>
-      <c r="J74" s="24" t="s">
-        <v>590</v>
-      </c>
+      <c r="I74" s="10"/>
+      <c r="J74" s="24"/>
       <c r="K74" s="9"/>
     </row>
     <row r="75" spans="1:11" ht="13">
@@ -12750,29 +12725,29 @@
         <v>132</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>233</v>
+        <v>214</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>215</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>411</v>
+        <v>47</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
       <c r="H75" s="9"/>
       <c r="I75" s="10" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="J75" s="24" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
       <c r="K75" s="9"/>
     </row>
@@ -12781,29 +12756,29 @@
         <v>132</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C76" s="9" t="s">
-        <v>381</v>
+        <v>214</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>382</v>
+        <v>157</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>593</v>
+        <v>219</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>594</v>
+        <v>575</v>
       </c>
       <c r="H76" s="9"/>
-      <c r="I76" s="11" t="s">
-        <v>595</v>
+      <c r="I76" s="10" t="s">
+        <v>220</v>
       </c>
       <c r="J76" s="24" t="s">
-        <v>596</v>
+        <v>576</v>
       </c>
       <c r="K76" s="9"/>
     </row>
@@ -12812,10 +12787,10 @@
         <v>132</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C77" s="9" t="s">
-        <v>237</v>
+        <v>221</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>577</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>411</v>
@@ -12824,17 +12799,17 @@
         <v>25</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>597</v>
+        <v>578</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="10" t="s">
-        <v>239</v>
+        <v>579</v>
       </c>
       <c r="J77" s="24" t="s">
-        <v>598</v>
+        <v>580</v>
       </c>
       <c r="K77" s="9"/>
     </row>
@@ -12843,29 +12818,29 @@
         <v>132</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C78" s="9" t="s">
-        <v>240</v>
+        <v>225</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>226</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>241</v>
+        <v>419</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>599</v>
+        <v>581</v>
       </c>
       <c r="H78" s="9"/>
       <c r="I78" s="10" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="J78" s="24" t="s">
-        <v>600</v>
+        <v>582</v>
       </c>
       <c r="K78" s="9"/>
     </row>
@@ -12874,29 +12849,29 @@
         <v>132</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C79" s="9" t="s">
-        <v>245</v>
+        <v>225</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>229</v>
       </c>
       <c r="D79" s="9" t="s">
-        <v>241</v>
+        <v>411</v>
       </c>
       <c r="E79" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>601</v>
+        <v>583</v>
       </c>
       <c r="H79" s="9"/>
       <c r="I79" s="10" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="J79" s="24" t="s">
-        <v>602</v>
+        <v>584</v>
       </c>
       <c r="K79" s="9"/>
     </row>
@@ -12905,29 +12880,29 @@
         <v>132</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>248</v>
+        <v>585</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>381</v>
+        <v>586</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>382</v>
+        <v>411</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>603</v>
+        <v>587</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>604</v>
+        <v>588</v>
       </c>
       <c r="H80" s="9"/>
-      <c r="I80" s="10" t="s">
-        <v>605</v>
+      <c r="I80" s="11" t="s">
+        <v>589</v>
       </c>
       <c r="J80" s="24" t="s">
-        <v>606</v>
+        <v>590</v>
       </c>
       <c r="K80" s="9"/>
     </row>
@@ -12936,29 +12911,29 @@
         <v>132</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>117</v>
+        <v>411</v>
       </c>
       <c r="E81" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>607</v>
+        <v>591</v>
       </c>
       <c r="H81" s="9"/>
       <c r="I81" s="10" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="J81" s="24" t="s">
-        <v>608</v>
+        <v>592</v>
       </c>
       <c r="K81" s="9"/>
     </row>
@@ -12967,29 +12942,29 @@
         <v>132</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>252</v>
+        <v>381</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>411</v>
+        <v>382</v>
       </c>
       <c r="E82" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>253</v>
+        <v>593</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>609</v>
+        <v>594</v>
       </c>
       <c r="H82" s="9"/>
-      <c r="I82" s="10" t="s">
-        <v>254</v>
+      <c r="I82" s="11" t="s">
+        <v>595</v>
       </c>
       <c r="J82" s="24" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="K82" s="9"/>
     </row>
@@ -12998,29 +12973,29 @@
         <v>132</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>117</v>
+        <v>411</v>
       </c>
       <c r="E83" s="9" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="H83" s="9"/>
       <c r="I83" s="10" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="J83" s="24" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="K83" s="9"/>
     </row>
@@ -13029,29 +13004,29 @@
         <v>132</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>259</v>
+        <v>240</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>117</v>
+        <v>241</v>
       </c>
       <c r="E84" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="H84" s="9"/>
       <c r="I84" s="10" t="s">
-        <v>261</v>
+        <v>243</v>
       </c>
       <c r="J84" s="24" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="K84" s="9"/>
     </row>
@@ -13060,29 +13035,29 @@
         <v>132</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>615</v>
+        <v>241</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>265</v>
+        <v>246</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>616</v>
+        <v>601</v>
       </c>
       <c r="H85" s="9"/>
-      <c r="I85" s="11" t="s">
-        <v>266</v>
+      <c r="I85" s="10" t="s">
+        <v>247</v>
       </c>
       <c r="J85" s="24" t="s">
-        <v>617</v>
+        <v>602</v>
       </c>
       <c r="K85" s="9"/>
     </row>
@@ -13091,29 +13066,29 @@
         <v>132</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>267</v>
+        <v>381</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>411</v>
+        <v>382</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>268</v>
+        <v>603</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="H86" s="9"/>
-      <c r="I86" s="11" t="s">
-        <v>269</v>
+      <c r="I86" s="10" t="s">
+        <v>605</v>
       </c>
       <c r="J86" s="24" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="K86" s="9"/>
     </row>
@@ -13122,29 +13097,29 @@
         <v>132</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>419</v>
+        <v>117</v>
       </c>
       <c r="E87" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="H87" s="9"/>
-      <c r="I87" s="11" t="s">
-        <v>272</v>
+      <c r="I87" s="10" t="s">
+        <v>251</v>
       </c>
       <c r="J87" s="24" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="K87" s="9"/>
     </row>
@@ -13153,29 +13128,29 @@
         <v>132</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>615</v>
+        <v>411</v>
       </c>
       <c r="E88" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="H88" s="9"/>
-      <c r="I88" s="11" t="s">
-        <v>275</v>
+      <c r="I88" s="10" t="s">
+        <v>254</v>
       </c>
       <c r="J88" s="24" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="K88" s="9"/>
     </row>
@@ -13184,273 +13159,263 @@
         <v>132</v>
       </c>
       <c r="B89" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G89" s="9" t="s">
+        <v>611</v>
+      </c>
+      <c r="H89" s="9"/>
+      <c r="I89" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="J89" s="24" t="s">
+        <v>612</v>
+      </c>
+      <c r="K89" s="9"/>
+    </row>
+    <row r="90" spans="1:11" ht="13">
+      <c r="A90" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G90" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="H90" s="9"/>
+      <c r="I90" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="J90" s="24" t="s">
+        <v>614</v>
+      </c>
+      <c r="K90" s="9"/>
+    </row>
+    <row r="91" spans="1:11" ht="13">
+      <c r="A91" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B91" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="C89" s="9" t="s">
+      <c r="C91" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="G91" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="H91" s="9"/>
+      <c r="I91" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="J91" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="K91" s="9"/>
+    </row>
+    <row r="92" spans="1:11" ht="13">
+      <c r="A92" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G92" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="H92" s="9"/>
+      <c r="I92" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="J92" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="K92" s="9"/>
+    </row>
+    <row r="93" spans="1:11" ht="13">
+      <c r="A93" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="G93" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="H93" s="9"/>
+      <c r="I93" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="J93" s="24" t="s">
+        <v>621</v>
+      </c>
+      <c r="K93" s="9"/>
+    </row>
+    <row r="94" spans="1:11" ht="13">
+      <c r="A94" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="G94" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="H94" s="9"/>
+      <c r="I94" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="J94" s="24" t="s">
+        <v>623</v>
+      </c>
+      <c r="K94" s="9"/>
+    </row>
+    <row r="95" spans="1:11" ht="13">
+      <c r="A95" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="11"/>
+      <c r="J95" s="24"/>
+      <c r="K95" s="9"/>
+    </row>
+    <row r="96" spans="1:11" ht="13">
+      <c r="A96" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="D89" s="9" t="s">
+      <c r="D96" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="E89" s="9" t="s">
+      <c r="E96" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F89" s="9" t="s">
+      <c r="F96" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="G89" s="9" t="s">
+      <c r="G96" s="9" t="s">
         <v>624</v>
       </c>
-      <c r="H89" s="9"/>
-      <c r="I89" s="11" t="s">
+      <c r="H96" s="9"/>
+      <c r="I96" s="11" t="s">
         <v>625</v>
       </c>
-      <c r="J89" s="24"/>
-      <c r="K89" s="9"/>
-    </row>
-    <row r="90" spans="1:11" ht="13">
-      <c r="A90" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>626</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>627</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E90" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F90" s="14" t="s">
-        <v>628</v>
-      </c>
-      <c r="G90" s="14" t="s">
-        <v>629</v>
-      </c>
-      <c r="H90" s="14"/>
-      <c r="I90" s="16" t="s">
-        <v>630</v>
-      </c>
-      <c r="J90" s="25" t="s">
-        <v>631</v>
-      </c>
-      <c r="K90" s="14"/>
-    </row>
-    <row r="91" spans="1:11" ht="13">
-      <c r="A91" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>626</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="E91" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>633</v>
-      </c>
-      <c r="G91" s="14" t="s">
-        <v>634</v>
-      </c>
-      <c r="H91" s="14"/>
-      <c r="I91" s="16" t="s">
-        <v>635</v>
-      </c>
-      <c r="J91" s="25" t="s">
-        <v>636</v>
-      </c>
-      <c r="K91" s="14"/>
-    </row>
-    <row r="92" spans="1:11" ht="13">
-      <c r="A92" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>637</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E92" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F92" s="14" t="s">
-        <v>638</v>
-      </c>
-      <c r="G92" s="14" t="s">
-        <v>639</v>
-      </c>
-      <c r="H92" s="14"/>
-      <c r="I92" s="15" t="s">
-        <v>640</v>
-      </c>
-      <c r="J92" s="25" t="s">
-        <v>641</v>
-      </c>
-      <c r="K92" s="14"/>
-    </row>
-    <row r="93" spans="1:11" ht="13">
-      <c r="A93" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>642</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F93" s="14" t="s">
-        <v>643</v>
-      </c>
-      <c r="G93" s="14" t="s">
-        <v>644</v>
-      </c>
-      <c r="H93" s="14"/>
-      <c r="I93" s="15" t="s">
-        <v>645</v>
-      </c>
-      <c r="J93" s="25" t="s">
-        <v>646</v>
-      </c>
-      <c r="K93" s="14"/>
-    </row>
-    <row r="94" spans="1:11" ht="13">
-      <c r="A94" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>647</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="E94" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F94" s="14" t="s">
-        <v>648</v>
-      </c>
-      <c r="G94" s="14" t="s">
-        <v>649</v>
-      </c>
-      <c r="H94" s="14"/>
-      <c r="I94" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="J94" s="25" t="s">
-        <v>651</v>
-      </c>
-      <c r="K94" s="14"/>
-    </row>
-    <row r="95" spans="1:11" ht="13">
-      <c r="A95" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>382</v>
-      </c>
-      <c r="E95" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F95" s="14" t="s">
-        <v>652</v>
-      </c>
-      <c r="G95" s="14" t="s">
-        <v>653</v>
-      </c>
-      <c r="H95" s="14"/>
-      <c r="I95" s="15" t="s">
-        <v>654</v>
-      </c>
-      <c r="J95" s="25"/>
-      <c r="K95" s="14"/>
-    </row>
-    <row r="96" spans="1:11" ht="13">
-      <c r="A96" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F96" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="G96" s="14" t="s">
-        <v>655</v>
-      </c>
-      <c r="H96" s="14"/>
-      <c r="I96" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="J96" s="25" t="s">
-        <v>656</v>
-      </c>
-      <c r="K96" s="14"/>
+      <c r="J96" s="24"/>
+      <c r="K96" s="9"/>
     </row>
     <row r="97" spans="1:11" ht="13">
       <c r="A97" s="14" t="s">
         <v>278</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>279</v>
+        <v>626</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>283</v>
+        <v>627</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>411</v>
+        <v>157</v>
       </c>
       <c r="E97" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F97" s="14" t="s">
-        <v>284</v>
+        <v>628</v>
       </c>
       <c r="G97" s="14" t="s">
-        <v>657</v>
+        <v>629</v>
       </c>
       <c r="H97" s="14"/>
-      <c r="I97" s="15" t="s">
-        <v>285</v>
+      <c r="I97" s="16" t="s">
+        <v>630</v>
       </c>
       <c r="J97" s="25" t="s">
-        <v>658</v>
+        <v>631</v>
       </c>
       <c r="K97" s="14"/>
     </row>
@@ -13459,29 +13424,29 @@
         <v>278</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>279</v>
+        <v>626</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>286</v>
+        <v>632</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F98" s="14" t="s">
-        <v>287</v>
+        <v>633</v>
       </c>
       <c r="G98" s="14" t="s">
-        <v>659</v>
+        <v>634</v>
       </c>
       <c r="H98" s="14"/>
       <c r="I98" s="16" t="s">
-        <v>288</v>
+        <v>635</v>
       </c>
       <c r="J98" s="25" t="s">
-        <v>660</v>
+        <v>636</v>
       </c>
       <c r="K98" s="14"/>
     </row>
@@ -13493,26 +13458,26 @@
         <v>279</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>289</v>
+        <v>637</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>290</v>
+        <v>638</v>
       </c>
       <c r="G99" s="14" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
       <c r="H99" s="14"/>
-      <c r="I99" s="16" t="s">
-        <v>291</v>
+      <c r="I99" s="15" t="s">
+        <v>640</v>
       </c>
       <c r="J99" s="25" t="s">
-        <v>662</v>
+        <v>641</v>
       </c>
       <c r="K99" s="14"/>
     </row>
@@ -13524,26 +13489,26 @@
         <v>279</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>292</v>
+        <v>642</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="E100" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>293</v>
+        <v>643</v>
       </c>
       <c r="G100" s="14" t="s">
-        <v>663</v>
+        <v>644</v>
       </c>
       <c r="H100" s="14"/>
-      <c r="I100" s="16" t="s">
-        <v>294</v>
+      <c r="I100" s="15" t="s">
+        <v>645</v>
       </c>
       <c r="J100" s="25" t="s">
-        <v>664</v>
+        <v>646</v>
       </c>
       <c r="K100" s="14"/>
     </row>
@@ -13555,7 +13520,7 @@
         <v>279</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>295</v>
+        <v>647</v>
       </c>
       <c r="D101" s="14" t="s">
         <v>411</v>
@@ -13564,17 +13529,17 @@
         <v>25</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>296</v>
+        <v>648</v>
       </c>
       <c r="G101" s="14" t="s">
-        <v>665</v>
+        <v>649</v>
       </c>
       <c r="H101" s="14"/>
-      <c r="I101" s="16" t="s">
-        <v>297</v>
+      <c r="I101" s="15" t="s">
+        <v>650</v>
       </c>
       <c r="J101" s="25" t="s">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="K101" s="14"/>
     </row>
@@ -13586,27 +13551,25 @@
         <v>279</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>298</v>
+        <v>381</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>411</v>
+        <v>382</v>
       </c>
       <c r="E102" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>299</v>
+        <v>652</v>
       </c>
       <c r="G102" s="14" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="H102" s="14"/>
-      <c r="I102" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="J102" s="25" t="s">
-        <v>668</v>
-      </c>
+      <c r="I102" s="15" t="s">
+        <v>654</v>
+      </c>
+      <c r="J102" s="25"/>
       <c r="K102" s="14"/>
     </row>
     <row r="103" spans="1:11" ht="13">
@@ -13614,29 +13577,29 @@
         <v>278</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>302</v>
+        <v>280</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="E103" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>303</v>
+        <v>281</v>
       </c>
       <c r="G103" s="14" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="H103" s="14"/>
       <c r="I103" s="15" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
       <c r="J103" s="25" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
       <c r="K103" s="14"/>
     </row>
@@ -13645,29 +13608,29 @@
         <v>278</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>381</v>
+        <v>283</v>
       </c>
       <c r="D104" s="14" t="s">
-        <v>382</v>
+        <v>411</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>671</v>
+        <v>284</v>
       </c>
       <c r="G104" s="14" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
       <c r="H104" s="14"/>
       <c r="I104" s="15" t="s">
-        <v>673</v>
+        <v>285</v>
       </c>
       <c r="J104" s="25" t="s">
-        <v>674</v>
+        <v>658</v>
       </c>
       <c r="K104" s="14"/>
     </row>
@@ -13676,29 +13639,29 @@
         <v>278</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>411</v>
+        <v>419</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="G105" s="14" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
       <c r="H105" s="14"/>
-      <c r="I105" s="15" t="s">
-        <v>308</v>
+      <c r="I105" s="16" t="s">
+        <v>288</v>
       </c>
       <c r="J105" s="25" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
       <c r="K105" s="14"/>
     </row>
@@ -13707,29 +13670,29 @@
         <v>278</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>411</v>
+        <v>117</v>
       </c>
       <c r="E106" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="G106" s="14" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="H106" s="14"/>
-      <c r="I106" s="15" t="s">
-        <v>310</v>
+      <c r="I106" s="16" t="s">
+        <v>291</v>
       </c>
       <c r="J106" s="25" t="s">
-        <v>678</v>
+        <v>662</v>
       </c>
       <c r="K106" s="14"/>
     </row>
@@ -13738,29 +13701,29 @@
         <v>278</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>305</v>
+        <v>279</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>312</v>
+        <v>47</v>
       </c>
       <c r="E107" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="G107" s="14" t="s">
-        <v>679</v>
+        <v>663</v>
       </c>
       <c r="H107" s="14"/>
-      <c r="I107" s="15" t="s">
-        <v>314</v>
+      <c r="I107" s="16" t="s">
+        <v>294</v>
       </c>
       <c r="J107" s="25" t="s">
-        <v>680</v>
+        <v>664</v>
       </c>
       <c r="K107" s="14"/>
     </row>
@@ -13769,10 +13732,10 @@
         <v>278</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="D108" s="14" t="s">
         <v>411</v>
@@ -13781,17 +13744,17 @@
         <v>25</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="G108" s="14" t="s">
-        <v>681</v>
+        <v>665</v>
       </c>
       <c r="H108" s="14"/>
-      <c r="I108" s="15" t="s">
-        <v>318</v>
+      <c r="I108" s="16" t="s">
+        <v>297</v>
       </c>
       <c r="J108" s="25" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
       <c r="K108" s="14"/>
     </row>
@@ -13800,29 +13763,29 @@
         <v>278</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="D109" s="14" t="s">
         <v>411</v>
       </c>
       <c r="E109" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>683</v>
+        <v>299</v>
       </c>
       <c r="G109" s="14" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
       <c r="H109" s="14"/>
       <c r="I109" s="16" t="s">
-        <v>685</v>
+        <v>300</v>
       </c>
       <c r="J109" s="25" t="s">
-        <v>686</v>
+        <v>668</v>
       </c>
       <c r="K109" s="14"/>
     </row>
@@ -13831,30 +13794,18 @@
         <v>278</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="E110" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F110" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="G110" s="14" t="s">
-        <v>687</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
       <c r="H110" s="14"/>
-      <c r="I110" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="J110" s="25" t="s">
-        <v>688</v>
-      </c>
+      <c r="I110" s="16"/>
+      <c r="J110" s="25"/>
       <c r="K110" s="14"/>
     </row>
     <row r="111" spans="1:11" ht="13">
@@ -13862,29 +13813,29 @@
         <v>278</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>689</v>
+        <v>302</v>
       </c>
       <c r="D111" s="14" t="s">
-        <v>411</v>
+        <v>117</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="G111" s="14" t="s">
-        <v>690</v>
+        <v>669</v>
       </c>
       <c r="H111" s="14"/>
       <c r="I111" s="15" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="J111" s="25" t="s">
-        <v>691</v>
+        <v>670</v>
       </c>
       <c r="K111" s="14"/>
     </row>
@@ -13893,29 +13844,29 @@
         <v>278</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>167</v>
+        <v>381</v>
       </c>
       <c r="D112" s="14" t="s">
-        <v>411</v>
+        <v>382</v>
       </c>
       <c r="E112" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F112" s="14" t="s">
-        <v>330</v>
+        <v>671</v>
       </c>
       <c r="G112" s="14" t="s">
-        <v>692</v>
+        <v>672</v>
       </c>
       <c r="H112" s="14"/>
       <c r="I112" s="15" t="s">
-        <v>331</v>
+        <v>673</v>
       </c>
       <c r="J112" s="25" t="s">
-        <v>693</v>
+        <v>674</v>
       </c>
       <c r="K112" s="14"/>
     </row>
@@ -13924,29 +13875,29 @@
         <v>278</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>332</v>
+        <v>306</v>
       </c>
       <c r="D113" s="14" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E113" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>333</v>
+        <v>307</v>
       </c>
       <c r="G113" s="14" t="s">
-        <v>694</v>
+        <v>675</v>
       </c>
       <c r="H113" s="14"/>
       <c r="I113" s="15" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="J113" s="25" t="s">
-        <v>695</v>
+        <v>676</v>
       </c>
       <c r="K113" s="14"/>
     </row>
@@ -13955,29 +13906,29 @@
         <v>278</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>47</v>
+        <v>411</v>
       </c>
       <c r="E114" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>336</v>
+        <v>309</v>
       </c>
       <c r="G114" s="14" t="s">
-        <v>696</v>
+        <v>677</v>
       </c>
       <c r="H114" s="14"/>
       <c r="I114" s="15" t="s">
-        <v>337</v>
+        <v>310</v>
       </c>
       <c r="J114" s="25" t="s">
-        <v>697</v>
+        <v>678</v>
       </c>
       <c r="K114" s="14"/>
     </row>
@@ -13986,29 +13937,29 @@
         <v>278</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="D115" s="14" t="s">
-        <v>117</v>
+        <v>312</v>
       </c>
       <c r="E115" s="14" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F115" s="14" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="G115" s="14" t="s">
-        <v>698</v>
+        <v>679</v>
       </c>
       <c r="H115" s="14"/>
       <c r="I115" s="15" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="J115" s="25" t="s">
-        <v>699</v>
+        <v>680</v>
       </c>
       <c r="K115" s="14"/>
     </row>
@@ -14017,30 +13968,18 @@
         <v>278</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="E116" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F116" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="G116" s="14" t="s">
-        <v>700</v>
-      </c>
+        <v>731</v>
+      </c>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
       <c r="H116" s="14"/>
-      <c r="I116" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="J116" s="25" t="s">
-        <v>701</v>
-      </c>
+      <c r="I116" s="15"/>
+      <c r="J116" s="25"/>
       <c r="K116" s="14"/>
     </row>
     <row r="117" spans="1:11" ht="13">
@@ -14048,29 +13987,29 @@
         <v>278</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="C117" s="14" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>47</v>
+        <v>411</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
       <c r="G117" s="14" t="s">
-        <v>702</v>
+        <v>681</v>
       </c>
       <c r="H117" s="14"/>
       <c r="I117" s="15" t="s">
-        <v>347</v>
+        <v>318</v>
       </c>
       <c r="J117" s="25" t="s">
-        <v>703</v>
+        <v>682</v>
       </c>
       <c r="K117" s="14"/>
     </row>
@@ -14079,30 +14018,18 @@
         <v>278</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>348</v>
+        <v>315</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E118" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F118" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="G118" s="14" t="s">
-        <v>704</v>
-      </c>
+        <v>722</v>
+      </c>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="14"/>
       <c r="H118" s="14"/>
-      <c r="I118" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="J118" s="25" t="s">
-        <v>705</v>
-      </c>
+      <c r="I118" s="15"/>
+      <c r="J118" s="25"/>
       <c r="K118" s="14"/>
     </row>
     <row r="119" spans="1:11" ht="13">
@@ -14110,29 +14037,29 @@
         <v>278</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>706</v>
+        <v>320</v>
       </c>
       <c r="D119" s="14" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="E119" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>353</v>
+        <v>683</v>
       </c>
       <c r="G119" s="14" t="s">
-        <v>707</v>
+        <v>684</v>
       </c>
       <c r="H119" s="14"/>
       <c r="I119" s="16" t="s">
-        <v>354</v>
+        <v>685</v>
       </c>
       <c r="J119" s="25" t="s">
-        <v>708</v>
+        <v>686</v>
       </c>
       <c r="K119" s="14"/>
     </row>
@@ -14141,29 +14068,29 @@
         <v>278</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>302</v>
+        <v>323</v>
       </c>
       <c r="D120" s="14" t="s">
-        <v>117</v>
+        <v>411</v>
       </c>
       <c r="E120" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="G120" s="14" t="s">
-        <v>709</v>
+        <v>687</v>
       </c>
       <c r="H120" s="14"/>
       <c r="I120" s="15" t="s">
-        <v>357</v>
+        <v>325</v>
       </c>
       <c r="J120" s="25" t="s">
-        <v>710</v>
+        <v>688</v>
       </c>
       <c r="K120" s="14"/>
     </row>
@@ -14172,29 +14099,29 @@
         <v>278</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>358</v>
+        <v>689</v>
       </c>
       <c r="D121" s="14" t="s">
         <v>411</v>
       </c>
       <c r="E121" s="14" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="G121" s="14" t="s">
-        <v>711</v>
+        <v>690</v>
       </c>
       <c r="H121" s="14"/>
       <c r="I121" s="15" t="s">
-        <v>360</v>
+        <v>328</v>
       </c>
       <c r="J121" s="25" t="s">
-        <v>712</v>
+        <v>691</v>
       </c>
       <c r="K121" s="14"/>
     </row>
@@ -14203,10 +14130,10 @@
         <v>278</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>713</v>
-      </c>
-      <c r="C122" s="17" t="s">
-        <v>714</v>
+        <v>329</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>167</v>
       </c>
       <c r="D122" s="14" t="s">
         <v>411</v>
@@ -14215,17 +14142,17 @@
         <v>25</v>
       </c>
       <c r="F122" s="14" t="s">
-        <v>715</v>
+        <v>330</v>
       </c>
       <c r="G122" s="14" t="s">
-        <v>716</v>
+        <v>692</v>
       </c>
       <c r="H122" s="14"/>
       <c r="I122" s="15" t="s">
-        <v>717</v>
+        <v>331</v>
       </c>
       <c r="J122" s="25" t="s">
-        <v>718</v>
+        <v>693</v>
       </c>
       <c r="K122" s="14"/>
     </row>
@@ -14234,10 +14161,10 @@
         <v>278</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>361</v>
-      </c>
-      <c r="C123" s="17" t="s">
-        <v>362</v>
+        <v>329</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>332</v>
       </c>
       <c r="D123" s="14" t="s">
         <v>419</v>
@@ -14246,19 +14173,353 @@
         <v>14</v>
       </c>
       <c r="F123" s="14" t="s">
-        <v>363</v>
+        <v>333</v>
       </c>
       <c r="G123" s="14" t="s">
-        <v>719</v>
+        <v>694</v>
       </c>
       <c r="H123" s="14"/>
       <c r="I123" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="J123" s="25" t="s">
+        <v>695</v>
+      </c>
+      <c r="K123" s="14"/>
+    </row>
+    <row r="124" spans="1:11" ht="13">
+      <c r="A124" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="D124" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F124" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="G124" s="14" t="s">
+        <v>696</v>
+      </c>
+      <c r="H124" s="14"/>
+      <c r="I124" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="J124" s="25" t="s">
+        <v>697</v>
+      </c>
+      <c r="K124" s="14"/>
+    </row>
+    <row r="125" spans="1:11" ht="13">
+      <c r="A125" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F125" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="G125" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="H125" s="14"/>
+      <c r="I125" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="J125" s="25" t="s">
+        <v>699</v>
+      </c>
+      <c r="K125" s="14"/>
+    </row>
+    <row r="126" spans="1:11" ht="13">
+      <c r="A126" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="E126" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F126" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="G126" s="14" t="s">
+        <v>700</v>
+      </c>
+      <c r="H126" s="14"/>
+      <c r="I126" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="J126" s="25" t="s">
+        <v>701</v>
+      </c>
+      <c r="K126" s="14"/>
+    </row>
+    <row r="127" spans="1:11" ht="13">
+      <c r="A127" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F127" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="G127" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="H127" s="14"/>
+      <c r="I127" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="J127" s="25" t="s">
+        <v>703</v>
+      </c>
+      <c r="K127" s="14"/>
+    </row>
+    <row r="128" spans="1:11" ht="13">
+      <c r="A128" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C128" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E128" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F128" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="G128" s="14" t="s">
+        <v>704</v>
+      </c>
+      <c r="H128" s="14"/>
+      <c r="I128" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="J128" s="25" t="s">
+        <v>705</v>
+      </c>
+      <c r="K128" s="14"/>
+    </row>
+    <row r="129" spans="1:11" ht="13">
+      <c r="A129" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C129" s="14" t="s">
+        <v>706</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="E129" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F129" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="G129" s="14" t="s">
+        <v>707</v>
+      </c>
+      <c r="H129" s="14"/>
+      <c r="I129" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="J129" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="K129" s="14"/>
+    </row>
+    <row r="130" spans="1:11" ht="13">
+      <c r="A130" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C130" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D130" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E130" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F130" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="G130" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="H130" s="14"/>
+      <c r="I130" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="J130" s="25" t="s">
+        <v>710</v>
+      </c>
+      <c r="K130" s="14"/>
+    </row>
+    <row r="131" spans="1:11" ht="13">
+      <c r="A131" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C131" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="D131" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="E131" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F131" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="G131" s="14" t="s">
+        <v>711</v>
+      </c>
+      <c r="H131" s="14"/>
+      <c r="I131" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="J131" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="K131" s="14"/>
+    </row>
+    <row r="132" spans="1:11" ht="13">
+      <c r="A132" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="D132" s="14"/>
+      <c r="E132" s="14"/>
+      <c r="F132" s="14"/>
+      <c r="G132" s="14"/>
+      <c r="H132" s="14"/>
+      <c r="I132" s="15"/>
+      <c r="J132" s="25"/>
+      <c r="K132" s="14"/>
+    </row>
+    <row r="133" spans="1:11" ht="13">
+      <c r="A133" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="C133" s="17" t="s">
+        <v>714</v>
+      </c>
+      <c r="D133" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="E133" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>715</v>
+      </c>
+      <c r="G133" s="14" t="s">
+        <v>716</v>
+      </c>
+      <c r="H133" s="14"/>
+      <c r="I133" s="15" t="s">
+        <v>717</v>
+      </c>
+      <c r="J133" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="K133" s="14"/>
+    </row>
+    <row r="134" spans="1:11" ht="13">
+      <c r="A134" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C134" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="D134" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="E134" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F134" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="G134" s="14" t="s">
+        <v>719</v>
+      </c>
+      <c r="H134" s="14"/>
+      <c r="I134" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="J123" s="25" t="s">
+      <c r="J134" s="25" t="s">
         <v>720</v>
       </c>
-      <c r="K123" s="14"/>
+      <c r="K134" s="14"/>
+    </row>
+    <row r="135" spans="1:11" ht="15.75" customHeight="1">
+      <c r="C135" s="14" t="s">
+        <v>727</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -14277,113 +14538,113 @@
     <hyperlink ref="I14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
     <hyperlink ref="I15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
     <hyperlink ref="I16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="I17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="I18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="I19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="I20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="I21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="I22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="I23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="I24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="I25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="I26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="I27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="I28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="I29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="I30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="I31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="I32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="I33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="I34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="I35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="I36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="I37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="I38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="I39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="I40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="I41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="I42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="I43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="I44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="I45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="I46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="I47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="I48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="I49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="I50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="I51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="I52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="I53" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="I54" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="I55" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="I56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="I57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="I58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="I59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="I60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="I61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="I62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="I63" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="I64" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="I65" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="I66" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="I67" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="I68" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
-    <hyperlink ref="I69" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
-    <hyperlink ref="I70" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
-    <hyperlink ref="I71" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
-    <hyperlink ref="I72" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
-    <hyperlink ref="I73" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
-    <hyperlink ref="I74" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
-    <hyperlink ref="I75" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
-    <hyperlink ref="I76" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
-    <hyperlink ref="I77" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
-    <hyperlink ref="I78" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
-    <hyperlink ref="I79" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
-    <hyperlink ref="I80" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
-    <hyperlink ref="I81" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
-    <hyperlink ref="I82" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
-    <hyperlink ref="I83" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
-    <hyperlink ref="I84" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
-    <hyperlink ref="I85" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
-    <hyperlink ref="I86" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
-    <hyperlink ref="I87" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
-    <hyperlink ref="I88" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
-    <hyperlink ref="I89" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
-    <hyperlink ref="I90" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
-    <hyperlink ref="I91" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
-    <hyperlink ref="I92" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
-    <hyperlink ref="I93" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
-    <hyperlink ref="I94" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
-    <hyperlink ref="I95" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
-    <hyperlink ref="I96" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
-    <hyperlink ref="I97" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
-    <hyperlink ref="I98" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
-    <hyperlink ref="I99" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
-    <hyperlink ref="I100" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
-    <hyperlink ref="I101" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
-    <hyperlink ref="I102" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
-    <hyperlink ref="I103" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
-    <hyperlink ref="I104" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
-    <hyperlink ref="I105" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
-    <hyperlink ref="I106" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
-    <hyperlink ref="I107" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
-    <hyperlink ref="I108" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
-    <hyperlink ref="I109" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
-    <hyperlink ref="I110" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
-    <hyperlink ref="I111" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
-    <hyperlink ref="I112" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
-    <hyperlink ref="I113" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
-    <hyperlink ref="I114" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
-    <hyperlink ref="I115" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
-    <hyperlink ref="I116" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
-    <hyperlink ref="I117" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
-    <hyperlink ref="I118" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
-    <hyperlink ref="I119" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
-    <hyperlink ref="I120" r:id="rId119" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
-    <hyperlink ref="I121" r:id="rId120" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
-    <hyperlink ref="I122" r:id="rId121" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
-    <hyperlink ref="I123" r:id="rId122" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
+    <hyperlink ref="I19" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="I20" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="I21" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="I22" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="I23" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="I24" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="I25" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="I26" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="I27" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="I28" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="I29" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="I30" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="I31" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="I32" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="I33" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="I34" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="I35" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="I38" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="I39" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="I40" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="I41" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="I42" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="I43" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="I44" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="I45" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="I46" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="I47" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="I48" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="I49" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="I50" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="I51" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="I52" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="I53" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="I54" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="I55" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="I56" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="I57" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="I58" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="I60" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="I61" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="I62" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="I63" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="I64" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="I65" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="I66" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="I67" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="I68" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="I69" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="I70" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="I71" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="I72" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="I73" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="I75" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="I76" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="I77" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="I78" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="I79" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="I80" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="I81" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="I82" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="I83" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="I84" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="I85" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="I86" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="I87" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="I88" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="I89" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="I90" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="I91" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="I92" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="I93" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
+    <hyperlink ref="I94" r:id="rId87" xr:uid="{00000000-0004-0000-0100-000056000000}"/>
+    <hyperlink ref="I96" r:id="rId88" xr:uid="{00000000-0004-0000-0100-000057000000}"/>
+    <hyperlink ref="I97" r:id="rId89" xr:uid="{00000000-0004-0000-0100-000058000000}"/>
+    <hyperlink ref="I98" r:id="rId90" xr:uid="{00000000-0004-0000-0100-000059000000}"/>
+    <hyperlink ref="I99" r:id="rId91" xr:uid="{00000000-0004-0000-0100-00005A000000}"/>
+    <hyperlink ref="I100" r:id="rId92" xr:uid="{00000000-0004-0000-0100-00005B000000}"/>
+    <hyperlink ref="I101" r:id="rId93" xr:uid="{00000000-0004-0000-0100-00005C000000}"/>
+    <hyperlink ref="I102" r:id="rId94" xr:uid="{00000000-0004-0000-0100-00005D000000}"/>
+    <hyperlink ref="I103" r:id="rId95" xr:uid="{00000000-0004-0000-0100-00005E000000}"/>
+    <hyperlink ref="I104" r:id="rId96" xr:uid="{00000000-0004-0000-0100-00005F000000}"/>
+    <hyperlink ref="I105" r:id="rId97" xr:uid="{00000000-0004-0000-0100-000060000000}"/>
+    <hyperlink ref="I106" r:id="rId98" xr:uid="{00000000-0004-0000-0100-000061000000}"/>
+    <hyperlink ref="I107" r:id="rId99" xr:uid="{00000000-0004-0000-0100-000062000000}"/>
+    <hyperlink ref="I108" r:id="rId100" xr:uid="{00000000-0004-0000-0100-000063000000}"/>
+    <hyperlink ref="I109" r:id="rId101" xr:uid="{00000000-0004-0000-0100-000064000000}"/>
+    <hyperlink ref="I111" r:id="rId102" xr:uid="{00000000-0004-0000-0100-000065000000}"/>
+    <hyperlink ref="I112" r:id="rId103" xr:uid="{00000000-0004-0000-0100-000066000000}"/>
+    <hyperlink ref="I113" r:id="rId104" xr:uid="{00000000-0004-0000-0100-000067000000}"/>
+    <hyperlink ref="I114" r:id="rId105" xr:uid="{00000000-0004-0000-0100-000068000000}"/>
+    <hyperlink ref="I115" r:id="rId106" xr:uid="{00000000-0004-0000-0100-000069000000}"/>
+    <hyperlink ref="I117" r:id="rId107" xr:uid="{00000000-0004-0000-0100-00006A000000}"/>
+    <hyperlink ref="I119" r:id="rId108" xr:uid="{00000000-0004-0000-0100-00006B000000}"/>
+    <hyperlink ref="I120" r:id="rId109" xr:uid="{00000000-0004-0000-0100-00006C000000}"/>
+    <hyperlink ref="I121" r:id="rId110" xr:uid="{00000000-0004-0000-0100-00006D000000}"/>
+    <hyperlink ref="I122" r:id="rId111" xr:uid="{00000000-0004-0000-0100-00006E000000}"/>
+    <hyperlink ref="I123" r:id="rId112" xr:uid="{00000000-0004-0000-0100-00006F000000}"/>
+    <hyperlink ref="I124" r:id="rId113" xr:uid="{00000000-0004-0000-0100-000070000000}"/>
+    <hyperlink ref="I125" r:id="rId114" xr:uid="{00000000-0004-0000-0100-000071000000}"/>
+    <hyperlink ref="I126" r:id="rId115" xr:uid="{00000000-0004-0000-0100-000072000000}"/>
+    <hyperlink ref="I127" r:id="rId116" xr:uid="{00000000-0004-0000-0100-000073000000}"/>
+    <hyperlink ref="I128" r:id="rId117" xr:uid="{00000000-0004-0000-0100-000074000000}"/>
+    <hyperlink ref="I129" r:id="rId118" xr:uid="{00000000-0004-0000-0100-000075000000}"/>
+    <hyperlink ref="I130" r:id="rId119" xr:uid="{00000000-0004-0000-0100-000076000000}"/>
+    <hyperlink ref="I131" r:id="rId120" xr:uid="{00000000-0004-0000-0100-000077000000}"/>
+    <hyperlink ref="I133" r:id="rId121" xr:uid="{00000000-0004-0000-0100-000078000000}"/>
+    <hyperlink ref="I134" r:id="rId122" xr:uid="{00000000-0004-0000-0100-000079000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>